<commit_message>
Fixed BOM for X3.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/production/BOM.xlsx
+++ b/Hardware/PCB/production/BOM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Downloads\device.faststepper_FORK-main (2)\device.faststepper_FORK-main\Hardware\PCB\production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\GitHub\open-ephys\device.faststepper\Hardware\PCB\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB89030-B04A-421A-8838-FAF28C0608B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AEA1A6-BE57-43F3-BB0C-34B121F9A5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C89F0AE-6C3B-47D9-B98F-AA927718F527}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C89F0AE-6C3B-47D9-B98F-AA927718F527}"/>
   </bookViews>
   <sheets>
     <sheet name="FastStepper" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">FastStepper!$A$1:$H$37</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">FastStepper!$A$1:$H$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="169">
   <si>
     <t>#</t>
   </si>
@@ -499,18 +499,6 @@
     <t>FastStepper PCBLib:90G-5</t>
   </si>
   <si>
-    <t>X3</t>
-  </si>
-  <si>
-    <t>conn 1x2</t>
-  </si>
-  <si>
-    <t>282834-2</t>
-  </si>
-  <si>
-    <t>OEPS070020</t>
-  </si>
-  <si>
     <t>FastStepper PCBLib:22-23-2031</t>
   </si>
   <si>
@@ -544,9 +532,6 @@
     <t>FastStepper PCBLib:22-23-2051</t>
   </si>
   <si>
-    <t>X4,X10</t>
-  </si>
-  <si>
     <t>conn 1x3</t>
   </si>
   <si>
@@ -566,6 +551,9 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>X3, X4,X10</t>
   </si>
 </sst>
 </file>
@@ -622,10 +610,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -686,8 +673,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85A68B4F-0192-487E-86D6-DF489B1F0BDE}" name="FastStepper" displayName="FastStepper" ref="A1:I37" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:I37" xr:uid="{85A68B4F-0192-487E-86D6-DF489B1F0BDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85A68B4F-0192-487E-86D6-DF489B1F0BDE}" name="FastStepper" displayName="FastStepper" ref="A1:I36" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I36" xr:uid="{85A68B4F-0192-487E-86D6-DF489B1F0BDE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3265AC52-AA63-4EA6-A549-BB0E5299BB31}" uniqueName="1" name="#" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{C5D6C42D-87A5-449E-AF3B-1BCF3C9E13C9}" uniqueName="2" name="Qty" queryTableFieldId="2"/>
@@ -1020,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42A423C-ABC3-4576-A226-F692314AE3A0}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1021,7 @@
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="91.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1065,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1075,26 +1062,26 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>169</v>
+      <c r="I2" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1104,26 +1091,26 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>169</v>
+      <c r="I3" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1133,26 +1120,26 @@
       <c r="B4">
         <v>29</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>169</v>
+      <c r="I4" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1162,26 +1149,26 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>169</v>
+      <c r="I5" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1191,26 +1178,26 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>169</v>
+      <c r="I6" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1220,26 +1207,26 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>169</v>
+      <c r="I7" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1249,26 +1236,26 @@
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>169</v>
+      <c r="I8" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1278,26 +1265,26 @@
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>169</v>
+      <c r="I9" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1307,26 +1294,26 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>169</v>
+      <c r="I10" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1336,26 +1323,26 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>169</v>
+      <c r="I11" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1365,26 +1352,26 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>169</v>
+      <c r="I12" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1394,26 +1381,26 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>169</v>
+      <c r="I13" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1423,26 +1410,26 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>169</v>
+      <c r="I14" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1452,26 +1439,26 @@
       <c r="B15">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>169</v>
+      <c r="I15" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1481,26 +1468,26 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" t="s">
         <v>76</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>170</v>
+      <c r="I16" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1510,26 +1497,26 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>169</v>
+      <c r="I17" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1539,26 +1526,26 @@
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>169</v>
+      <c r="I18" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1568,26 +1555,26 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>169</v>
+      <c r="I19" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1597,26 +1584,26 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" t="s">
         <v>94</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>169</v>
+      <c r="I20" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1626,26 +1613,26 @@
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" t="s">
         <v>98</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" t="s">
         <v>94</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>169</v>
+      <c r="I21" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1655,26 +1642,26 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>169</v>
+      <c r="I22" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1684,26 +1671,26 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" t="s">
         <v>106</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" t="s">
         <v>94</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>169</v>
+      <c r="I23" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1713,26 +1700,26 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>108</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
         <v>109</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" t="s">
         <v>110</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
         <v>94</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>169</v>
+      <c r="I24" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1742,26 +1729,26 @@
       <c r="B25">
         <v>3</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
         <v>113</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
         <v>94</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>169</v>
+      <c r="I25" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1771,26 +1758,26 @@
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>116</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" t="s">
         <v>118</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" t="s">
         <v>94</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>169</v>
+      <c r="I26" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1800,26 +1787,26 @@
       <c r="B27">
         <v>14</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>120</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
         <v>121</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" t="s">
         <v>122</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" t="s">
         <v>94</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>169</v>
+      <c r="I27" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1829,26 +1816,26 @@
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>124</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
         <v>125</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" t="s">
         <v>126</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" t="s">
         <v>127</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>169</v>
+      <c r="I28" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1858,26 +1845,26 @@
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>128</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
         <v>130</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" t="s">
         <v>131</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" t="s">
         <v>132</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>171</v>
+      <c r="I29" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1887,26 +1874,26 @@
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>133</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>134</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
         <v>135</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" t="s">
         <v>136</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" t="s">
         <v>137</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>169</v>
+      <c r="I30" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1916,26 +1903,26 @@
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>138</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
         <v>139</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" t="s">
         <v>140</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" t="s">
         <v>141</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>169</v>
+      <c r="I31" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1945,26 +1932,26 @@
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
         <v>143</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" t="s">
         <v>144</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" t="s">
         <v>141</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>169</v>
+      <c r="I32" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1974,26 +1961,26 @@
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>145</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>146</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" t="s">
         <v>148</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" t="s">
         <v>149</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>171</v>
+      <c r="I33" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2003,26 +1990,26 @@
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="C34" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="D34" t="s">
         <v>152</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
         <v>153</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="G34" t="s">
         <v>154</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>171</v>
+      <c r="H34" t="s">
+        <v>155</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2030,28 +2017,28 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
         <v>156</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="D35" t="s">
         <v>157</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
         <v>158</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="G35" t="s">
         <v>159</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>169</v>
+      <c r="H35" t="s">
+        <v>160</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2061,55 +2048,26 @@
       <c r="B36">
         <v>3</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" t="s">
         <v>161</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
         <v>162</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" t="s">
         <v>163</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="H36" t="s">
+        <v>150</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>